<commit_message>
20190707 done, 20190708 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chengxu\java\maven\crazyCodeLove.github.io\work\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B74771-F0A7-403D-8D43-A9D817605490}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19200" windowHeight="11625"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -78,8 +72,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,28 +88,345 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -117,9 +434,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -131,13 +690,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <i val="0"/>
       </font>
       <fill>
@@ -157,7 +764,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -165,9 +772,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -454,28 +1058,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.44166666666667" customWidth="1"/>
+    <col min="2" max="2" width="14.775" customWidth="1"/>
+    <col min="3" max="3" width="13.8833333333333" customWidth="1"/>
+    <col min="4" max="4" width="7.21666666666667" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +1126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>20190701</v>
       </c>
@@ -569,7 +1173,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>20190702</v>
       </c>
@@ -616,7 +1220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>20190703</v>
       </c>
@@ -663,7 +1267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>20190704</v>
       </c>
@@ -710,7 +1314,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>20190705</v>
       </c>
@@ -757,7 +1361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>20190706</v>
       </c>
@@ -804,42 +1408,95 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>20190707</v>
       </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>20190708</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20190708 done, 20190709 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -74,10 +74,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -90,6 +90,65 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,16 +177,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -136,21 +195,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,51 +217,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -241,6 +241,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -271,19 +343,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,72 +386,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,6 +432,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -455,6 +470,26 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -491,41 +526,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -540,10 +540,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,133 +552,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1064,10 +1064,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1431,7 +1431,7 @@
         <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
         <v>16</v>
@@ -1455,9 +1455,56 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>20190708</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>20190709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20190709 done, 20190710 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chengxu\java\maven\crazyCodeLove.github.io\work\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF289DB7-25EF-41C6-8557-E51F534EE7CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="11625"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -72,14 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,345 +88,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -434,251 +110,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -690,61 +124,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
       </font>
       <fill>
@@ -764,7 +150,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -772,6 +158,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1058,28 +447,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:O10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44166666666667" customWidth="1"/>
-    <col min="2" max="2" width="14.775" customWidth="1"/>
-    <col min="3" max="3" width="13.8833333333333" customWidth="1"/>
-    <col min="4" max="4" width="7.21666666666667" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:15">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +515,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20190701</v>
       </c>
@@ -1173,7 +562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20190702</v>
       </c>
@@ -1220,7 +609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20190703</v>
       </c>
@@ -1267,7 +656,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20190704</v>
       </c>
@@ -1314,7 +703,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20190705</v>
       </c>
@@ -1361,7 +750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20190706</v>
       </c>
@@ -1408,7 +797,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20190707</v>
       </c>
@@ -1455,7 +844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20190708</v>
       </c>
@@ -1502,48 +891,89 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20190709</v>
       </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20190710</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20190710 done, 20190711 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chengxu\java\maven\crazyCodeLove.github.io\work\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF289DB7-25EF-41C6-8557-E51F534EE7CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19200" windowHeight="11625"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -78,8 +72,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,21 +88,345 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -110,9 +434,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -124,13 +690,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <i val="0"/>
       </font>
       <fill>
@@ -150,7 +764,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -158,9 +772,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -447,28 +1058,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.44166666666667" customWidth="1"/>
+    <col min="2" max="2" width="14.775" customWidth="1"/>
+    <col min="3" max="3" width="13.8833333333333" customWidth="1"/>
+    <col min="4" max="4" width="7.21666666666667" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +1126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>20190701</v>
       </c>
@@ -562,7 +1173,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>20190702</v>
       </c>
@@ -609,7 +1220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>20190703</v>
       </c>
@@ -656,7 +1267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>20190704</v>
       </c>
@@ -703,7 +1314,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>20190705</v>
       </c>
@@ -750,7 +1361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>20190706</v>
       </c>
@@ -797,7 +1408,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>20190707</v>
       </c>
@@ -844,7 +1455,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>20190708</v>
       </c>
@@ -891,7 +1502,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>20190709</v>
       </c>
@@ -938,42 +1549,131 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>20190710</v>
       </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+      <c r="M11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12">
+        <v>20190711</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L12" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20190713 done， 20190714 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chengxu\java\maven\crazyCodeLove.github.io\work\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E0BC9F-4EE7-49E1-BABD-C0AE9C343D61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="11625"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -72,14 +78,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,345 +88,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -434,251 +117,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -690,61 +131,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <i val="0"/>
       </font>
       <fill>
@@ -764,7 +157,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -772,6 +165,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1058,28 +454,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:O12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44166666666667" customWidth="1"/>
-    <col min="2" max="2" width="14.775" customWidth="1"/>
-    <col min="3" max="3" width="13.8833333333333" customWidth="1"/>
-    <col min="4" max="4" width="7.21666666666667" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:15">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20190701</v>
       </c>
@@ -1173,7 +569,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20190702</v>
       </c>
@@ -1220,7 +616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20190703</v>
       </c>
@@ -1267,7 +663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20190704</v>
       </c>
@@ -1314,7 +710,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20190705</v>
       </c>
@@ -1361,7 +757,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>20190706</v>
       </c>
@@ -1408,7 +804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>20190707</v>
       </c>
@@ -1455,7 +851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>20190708</v>
       </c>
@@ -1502,7 +898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>20190709</v>
       </c>
@@ -1549,7 +945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20190710</v>
       </c>
@@ -1596,7 +992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20190711</v>
       </c>
@@ -1606,6 +1002,9 @@
       <c r="C12" t="s">
         <v>16</v>
       </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
       <c r="E12" t="s">
         <v>16</v>
       </c>
@@ -1615,6 +1014,9 @@
       <c r="G12" t="s">
         <v>16</v>
       </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
       <c r="I12" t="s">
         <v>16</v>
       </c>
@@ -1637,43 +1039,136 @@
         <v>16</v>
       </c>
     </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20190712</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" t="s">
+        <v>16</v>
+      </c>
+      <c r="O13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20190713</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+      <c r="L14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" t="s">
+        <v>16</v>
+      </c>
+      <c r="O14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20190714</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20190715 done, 20190716 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\chengxu\java\maven\crazyCodeLove.github.io\work\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E0BC9F-4EE7-49E1-BABD-C0AE9C343D61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="19200" windowHeight="11625"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -78,8 +72,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,28 +88,345 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -117,9 +434,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -131,13 +690,61 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <i val="0"/>
       </font>
       <fill>
@@ -157,7 +764,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -165,9 +772,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -454,28 +1058,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" customWidth="1"/>
+    <col min="1" max="1" width="9.44166666666667" customWidth="1"/>
+    <col min="2" max="2" width="14.775" customWidth="1"/>
+    <col min="3" max="3" width="13.8833333333333" customWidth="1"/>
+    <col min="4" max="4" width="7.21666666666667" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +1126,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>20190701</v>
       </c>
@@ -569,7 +1173,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>20190702</v>
       </c>
@@ -616,7 +1220,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>20190703</v>
       </c>
@@ -663,7 +1267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>20190704</v>
       </c>
@@ -710,7 +1314,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>20190705</v>
       </c>
@@ -757,7 +1361,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>20190706</v>
       </c>
@@ -804,7 +1408,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>20190707</v>
       </c>
@@ -851,7 +1455,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>20190708</v>
       </c>
@@ -898,7 +1502,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>20190709</v>
       </c>
@@ -945,7 +1549,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>20190710</v>
       </c>
@@ -992,7 +1596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>20190711</v>
       </c>
@@ -1039,7 +1643,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>20190712</v>
       </c>
@@ -1086,7 +1690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>20190713</v>
       </c>
@@ -1133,42 +1737,176 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>20190714</v>
       </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" t="s">
+        <v>16</v>
+      </c>
+      <c r="O15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16">
+        <v>20190715</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" t="s">
+        <v>16</v>
+      </c>
+      <c r="O16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>20190716</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17"/>
+      <c r="N17" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
20190716 done, 20190717 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -85,13 +85,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -210,6 +203,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -241,187 +241,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,10 +540,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,133 +552,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1064,10 +1064,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1831,7 +1831,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>20190716</v>
       </c>
@@ -1841,6 +1841,9 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
       <c r="E17" t="s">
         <v>16</v>
       </c>
@@ -1848,10 +1851,10 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I17" t="s">
         <v>16</v>
@@ -1865,8 +1868,42 @@
       <c r="L17" t="s">
         <v>16</v>
       </c>
-      <c r="M17"/>
+      <c r="M17" t="s">
+        <v>16</v>
+      </c>
       <c r="N17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18">
+        <v>20190717</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K18" t="s">
+        <v>16</v>
+      </c>
+      <c r="O18" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
20190717 done, 20190718 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -74,10 +74,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -85,6 +85,13 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -204,7 +211,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,20 +231,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -241,24 +241,78 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -271,25 +325,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,30 +391,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -343,85 +403,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,10 +540,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,133 +552,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1064,10 +1064,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1888,12 +1888,21 @@
       <c r="C18" t="s">
         <v>16</v>
       </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
       <c r="E18" t="s">
         <v>16</v>
       </c>
       <c r="F18" t="s">
         <v>16</v>
       </c>
+      <c r="G18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
       <c r="I18" t="s">
         <v>16</v>
       </c>
@@ -1903,7 +1912,27 @@
       <c r="K18" t="s">
         <v>16</v>
       </c>
+      <c r="L18" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" t="s">
+        <v>15</v>
+      </c>
+      <c r="N18" t="s">
+        <v>16</v>
+      </c>
       <c r="O18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19">
+        <v>20190718</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="O19" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
20190722 done, 20190723 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -103,9 +103,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -116,6 +131,14 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -135,14 +158,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -151,7 +174,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,21 +205,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,45 +219,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,31 +241,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,151 +415,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,17 +446,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,6 +489,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -518,15 +527,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -540,10 +540,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,133 +552,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1064,10 +1064,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2113,9 +2113,95 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:15">
       <c r="A23">
         <v>20190722</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" t="s">
+        <v>16</v>
+      </c>
+      <c r="K23" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" t="s">
+        <v>16</v>
+      </c>
+      <c r="N23" t="s">
+        <v>16</v>
+      </c>
+      <c r="O23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24">
+        <v>20190723</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M24" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24" t="s">
+        <v>16</v>
+      </c>
+      <c r="O24" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20190730 before done, 20190731 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -74,8 +74,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -90,6 +90,29 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -111,6 +134,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -119,7 +157,31 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -135,7 +197,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -149,46 +211,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,36 +231,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -247,181 +247,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,11 +435,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -461,9 +491,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -483,47 +524,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -540,10 +540,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,133 +552,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1064,10 +1064,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2258,9 +2258,15 @@
       <c r="A26">
         <v>20190725</v>
       </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
       <c r="C26" t="s">
         <v>16</v>
       </c>
+      <c r="D26" t="s">
+        <v>15</v>
+      </c>
       <c r="E26" t="s">
         <v>16</v>
       </c>
@@ -2270,6 +2276,9 @@
       <c r="G26" t="s">
         <v>16</v>
       </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
       <c r="I26" t="s">
         <v>16</v>
       </c>
@@ -2290,6 +2299,243 @@
       </c>
       <c r="O26" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27">
+        <v>20190726</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" t="s">
+        <v>16</v>
+      </c>
+      <c r="L27" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" t="s">
+        <v>16</v>
+      </c>
+      <c r="N27" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28">
+        <v>20190727</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" t="s">
+        <v>16</v>
+      </c>
+      <c r="N28" t="s">
+        <v>16</v>
+      </c>
+      <c r="O28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29">
+        <v>20190728</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" t="s">
+        <v>16</v>
+      </c>
+      <c r="J29" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" t="s">
+        <v>16</v>
+      </c>
+      <c r="L29" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" t="s">
+        <v>16</v>
+      </c>
+      <c r="N29" t="s">
+        <v>16</v>
+      </c>
+      <c r="O29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30">
+        <v>20190729</v>
+      </c>
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" t="s">
+        <v>16</v>
+      </c>
+      <c r="L30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" t="s">
+        <v>16</v>
+      </c>
+      <c r="O30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31">
+        <v>20190730</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" t="s">
+        <v>16</v>
+      </c>
+      <c r="J31" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" t="s">
+        <v>16</v>
+      </c>
+      <c r="L31" t="s">
+        <v>16</v>
+      </c>
+      <c r="M31" t="s">
+        <v>16</v>
+      </c>
+      <c r="N31" t="s">
+        <v>16</v>
+      </c>
+      <c r="O31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32">
+        <v>20190731</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20190808 befo done, 20190808 init
</commit_message>
<xml_diff>
--- a/work/检查列表2019.xlsx
+++ b/work/检查列表2019.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="17">
   <si>
     <t>时间</t>
   </si>
@@ -75,9 +75,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1064,10 +1064,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2530,12 +2530,159 @@
         <v>16</v>
       </c>
       <c r="O31" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32">
-        <v>20190731</v>
+        <v>20190805</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" t="s">
+        <v>16</v>
+      </c>
+      <c r="K32" t="s">
+        <v>16</v>
+      </c>
+      <c r="L32" t="s">
+        <v>16</v>
+      </c>
+      <c r="M32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N32" t="s">
+        <v>16</v>
+      </c>
+      <c r="O32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33">
+        <v>20190806</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" t="s">
+        <v>16</v>
+      </c>
+      <c r="I33" t="s">
+        <v>16</v>
+      </c>
+      <c r="J33" t="s">
+        <v>16</v>
+      </c>
+      <c r="K33" t="s">
+        <v>16</v>
+      </c>
+      <c r="L33" t="s">
+        <v>16</v>
+      </c>
+      <c r="M33" t="s">
+        <v>16</v>
+      </c>
+      <c r="N33" t="s">
+        <v>16</v>
+      </c>
+      <c r="O33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34">
+        <v>20190807</v>
+      </c>
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" t="s">
+        <v>16</v>
+      </c>
+      <c r="J34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K34" t="s">
+        <v>16</v>
+      </c>
+      <c r="L34" t="s">
+        <v>16</v>
+      </c>
+      <c r="M34" t="s">
+        <v>16</v>
+      </c>
+      <c r="N34" t="s">
+        <v>16</v>
+      </c>
+      <c r="O34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>20190808</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>